<commit_message>
obtained real data and processed/cleaned it
</commit_message>
<xml_diff>
--- a/CITATION_INFO.xlsx
+++ b/CITATION_INFO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjack\Desktop\Lakeland_Electric\Lakeland_Electric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CDFC44-8A13-418A-B99F-393AE93FF9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C10FB7-CE5B-4F8D-804D-EADF70E5C2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>